<commit_message>
feat: sheet single page done
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\KP\Software-SPMI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hafidz Raihan\PhpstormProjects\Software-SPMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C8A690-63DF-4D47-BE1F-9748ECC233DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380663A3-FCC3-4755-A652-975B57EE930F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1FCCA566-237F-4610-B2CE-383DE46F6AD8}"/>
   </bookViews>
@@ -16,26 +16,17 @@
     <sheet name="Table XI" sheetId="1" r:id="rId1"/>
     <sheet name="Table X" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
   <si>
     <t>PENETAPAN</t>
   </si>
@@ -223,17 +214,21 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4050F9A2-F2EA-4DF7-BE8C-E53944F916C1}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,247 +560,247 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
+      <c r="C4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
+      <c r="C5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
+      <c r="C6">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
+      <c r="C7">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
+      <c r="C8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
+      <c r="C9">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
-        <v>19</v>
+      <c r="C10">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
-        <v>20</v>
+      <c r="C11">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
-        <v>33</v>
+      <c r="C14">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
-        <v>34</v>
+      <c r="C15">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
-        <v>35</v>
+      <c r="C16">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
-        <v>36</v>
+      <c r="C17">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
-        <v>37</v>
+      <c r="C18">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="C19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="C21" t="s">
-        <v>33</v>
+      <c r="C21">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
-        <v>34</v>
+      <c r="C22">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1" t="s">
+      <c r="A23" s="2"/>
+      <c r="B23" t="s">
         <v>29</v>
       </c>
-      <c r="C23" t="s">
-        <v>35</v>
+      <c r="C23">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="2"/>
+      <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="C24" t="s">
-        <v>36</v>
+      <c r="C24">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="1" t="s">
+      <c r="A25" s="2"/>
+      <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
-        <v>37</v>
+      <c r="C25">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" t="s">
-        <v>38</v>
+      <c r="C26">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -844,45 +839,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
@@ -890,8 +885,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
@@ -899,8 +894,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
@@ -908,8 +903,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
@@ -917,10 +912,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
@@ -928,8 +923,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
@@ -937,10 +932,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
@@ -948,8 +943,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
@@ -957,24 +952,24 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>27</v>
       </c>
       <c r="C14" t="s">
@@ -982,8 +977,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" t="s">
         <v>28</v>
       </c>
       <c r="C15" t="s">
@@ -991,8 +986,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" t="s">
         <v>29</v>
       </c>
       <c r="C16" t="s">
@@ -1000,8 +995,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" t="s">
         <v>30</v>
       </c>
       <c r="C17" t="s">
@@ -1009,8 +1004,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" t="s">
         <v>31</v>
       </c>
       <c r="C18" t="s">
@@ -1018,24 +1013,24 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" t="s">
         <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>27</v>
       </c>
       <c r="C21" t="s">
@@ -1043,8 +1038,8 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" t="s">
         <v>28</v>
       </c>
       <c r="C22" t="s">
@@ -1052,8 +1047,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1" t="s">
+      <c r="A23" s="2"/>
+      <c r="B23" t="s">
         <v>29</v>
       </c>
       <c r="C23" t="s">
@@ -1061,8 +1056,8 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="2"/>
+      <c r="B24" t="s">
         <v>30</v>
       </c>
       <c r="C24" t="s">
@@ -1070,8 +1065,8 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="1" t="s">
+      <c r="A25" s="2"/>
+      <c r="B25" t="s">
         <v>31</v>
       </c>
       <c r="C25" t="s">
@@ -1079,8 +1074,8 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" t="s">
         <v>32</v>
       </c>
       <c r="C26" t="s">
@@ -1089,17 +1084,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:G2"/>
+    <mergeCell ref="A3:XFD3"/>
+    <mergeCell ref="A4:A7"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:XFD13"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:XFD20"/>
     <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:G2"/>
-    <mergeCell ref="A3:XFD3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
import multiple sheet done
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\KP\Software-SPMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8685067C-CFE7-4A4B-8A7A-200CF8A0FA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1BC4A0-B34B-41A8-BC16-B73C8B3D8B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1FCCA566-237F-4610-B2CE-383DE46F6AD8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table XI" sheetId="1" r:id="rId1"/>
-    <sheet name="Table X" sheetId="2" r:id="rId2"/>
+    <sheet name="Informatika" sheetId="1" r:id="rId1"/>
+    <sheet name="Elektro" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>PENETAPAN</t>
   </si>
@@ -67,21 +67,12 @@
     <t>INDIKATOR 9</t>
   </si>
   <si>
-    <t>STANDAR 1</t>
-  </si>
-  <si>
-    <t>STANDAR 2</t>
-  </si>
-  <si>
     <t>STANDAR 3</t>
   </si>
   <si>
     <t>INPUT</t>
   </si>
   <si>
-    <t>STANDAR 4</t>
-  </si>
-  <si>
     <t>INDIKATOR 10</t>
   </si>
   <si>
@@ -104,6 +95,30 @@
   </si>
   <si>
     <t>PROSES</t>
+  </si>
+  <si>
+    <t>Mampu Membobol System Google</t>
+  </si>
+  <si>
+    <t>Ahli Dalam Data Science</t>
+  </si>
+  <si>
+    <t>Bekerja Sesuai Bidang Minat</t>
+  </si>
+  <si>
+    <t>Menjadi CEO</t>
+  </si>
+  <si>
+    <t>Kebal Terhadapat Listrik Tegangan Tinggi</t>
+  </si>
+  <si>
+    <t>Mampu Membuat Panel Surya</t>
+  </si>
+  <si>
+    <t>Bisa Melawan Thor menggunakan palu Tukang</t>
+  </si>
+  <si>
+    <t>Bisa membuat robot</t>
   </si>
 </sst>
 </file>
@@ -158,6 +173,13 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -172,13 +194,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,13 +511,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4050F9A2-F2EA-4DF7-BE8C-E53944F916C1}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
@@ -510,15 +525,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -530,29 +545,29 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
+      <c r="A4" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -561,7 +576,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -570,7 +585,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -579,8 +594,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
+      <c r="A8" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -590,7 +605,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -599,8 +614,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
+      <c r="A10" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -610,7 +625,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -619,7 +634,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -627,123 +642,123 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="5"/>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>24</v>
+    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>17</v>
+      <c r="A21" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="5"/>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="5"/>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C23">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="5"/>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="5"/>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="A26" s="5"/>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -772,26 +787,26 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A14" sqref="A14:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -803,19 +818,19 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
+      <c r="A4" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -825,7 +840,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -834,7 +849,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -843,7 +858,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -852,8 +867,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
+      <c r="A8" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -863,7 +878,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -872,8 +887,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
+      <c r="A10" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -883,7 +898,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -892,7 +907,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -900,85 +915,85 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>25</v>
+    <row r="13" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
+      <c r="A14" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="5"/>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>